<commit_message>
removed self from staticmethod
</commit_message>
<xml_diff>
--- a/Yale.xlsx
+++ b/Yale.xlsx
@@ -30,7 +30,7 @@
       <sz val="24"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -55,12 +55,6 @@
         <bgColor rgb="00E1E4E5"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E06666"/>
-        <bgColor rgb="00E06666"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -81,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -97,9 +91,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -429,19 +420,19 @@
     <row r="2">
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>Turbo English - January</t>
+          <t>Turbo English - May</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>May</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="J3" t="inlineStr">
         <is>
-          <t>1 Classes</t>
+          <t>5 Classes</t>
         </is>
       </c>
     </row>
@@ -480,31 +471,31 @@
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>01/01</t>
+          <t>05/05</t>
         </is>
       </c>
       <c r="B6" s="3" t="n"/>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>01/02</t>
+          <t>05/06</t>
         </is>
       </c>
       <c r="D6" s="3" t="n"/>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>01/03</t>
+          <t>05/07</t>
         </is>
       </c>
       <c r="F6" s="3" t="n"/>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>01/04</t>
+          <t>05/08</t>
         </is>
       </c>
       <c r="H6" s="3" t="n"/>
       <c r="I6" s="4" t="inlineStr">
         <is>
-          <t>01/05</t>
+          <t>05/09</t>
         </is>
       </c>
       <c r="J6" s="3" t="n"/>
@@ -512,52 +503,64 @@
     <row r="7" ht="88.5" customHeight="1">
       <c r="A7" s="5" t="inlineStr">
         <is>
+          <t>Welome:
+Welcome
+4 - 7</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Workbook:
+p. 4 - 5
+ Study flashcards </t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Unit  1:
+In the Classroom
+8 - 11</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Workbook:
+p. 6 - 7
+ Study flashcards </t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>Unit  1:
+In the Classroom
+12 - 15</t>
+        </is>
+      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Workbook:
+p. 8 - 9
+ Study flashcards </t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="H7" s="6" t="inlineStr">
+        <is>
+          <t>Flashcards</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
           <t>Review</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="J7" s="6" t="inlineStr">
         <is>
           <t>Flashcards</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="D7" s="6" t="inlineStr">
-        <is>
-          <t>Flashcards</t>
-        </is>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>Flashcards</t>
-        </is>
-      </c>
-      <c r="G7" s="7" t="inlineStr">
-        <is>
-          <t>No School</t>
-        </is>
-      </c>
-      <c r="H7" s="6" t="inlineStr">
-        <is>
-          <t>No Homework</t>
-        </is>
-      </c>
-      <c r="I7" s="7" t="inlineStr">
-        <is>
-          <t>No School</t>
-        </is>
-      </c>
-      <c r="J7" s="6" t="inlineStr">
-        <is>
-          <t>No Homework</t>
         </is>
       </c>
     </row>
@@ -567,7 +570,7 @@
     <row r="19" ht="88.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C2:G3"/>
+    <mergeCell ref="C2:H3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C5:D5"/>

</xml_diff>